<commit_message>
- `Scenarios` excel file gets additional columns `SteadyStateTime`, `SteadyStateTimeUnit`, `PopulationId`. - `ScenarioConfiguration` gets a new field `populationId`, specifying the id of population as defined in the `PopulationParameters.xlsx` file, sheet `Demographics`. If the field is `NULL`, the scenario is simulated as an individual simulation, otherwise a population simulation is performed.
- `runScenraios()` supports scenario configurations for population simulations

- Target folder for saving `*.pkml` simulations when `runScenarios(scenarioConfigurations, saveSimulationsToPKML = TRUE)`
changed from `Models/Simulations/<DateSuffix>` to `Results/SimulationResults/<DateSuffix>`.
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/PopulationParameters.xlsx
+++ b/tests/data/TestProject/Parameters/PopulationParameters.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/Services/Freigegebene Dokumente/_Project_template_V02.00/WP1_V00.01/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_3A82F05DCDDED6DECC8108D2AAE166FCA5131A3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D9440E7-2BDE-40B7-BCBC-A35A92C4F916}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B8C94-13CA-4464-A6AD-FE203ECC14C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9190" yWindow="430" windowWidth="28800" windowHeight="15290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="UserDefinedVariability" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -450,26 +450,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -533,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -565,16 +564,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDC7527-4ED0-4425-B4F9-CA5C81A120DE}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -866,6 +865,8 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -879,5 +880,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B86647EE-866F-4D07-B65C-304BD8EB10F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B86647EE-866F-4D07-B65C-304BD8EB10F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- `Scenarios` excel file gets additional columns `SteadyStateTime`, `SteadyStateTimeUnit`, (#376)
`PopulationId`.
- `ScenarioConfiguration` gets a new field `populationId`, specifying the id of
population as defined in the `PopulationParameters.xlsx` file, sheet `Demographics`.
If the field is `NULL`, the scenario is simulated as an individual simulation,
otherwise a population simulation is performed.

- `runScenraios()` supports scenario configurations for population simulations

- Target folder for saving `*.pkml` simulations when `runScenarios(scenarioConfigurations, saveSimulationsToPKML = TRUE)`
changed from `Models/Simulations/<DateSuffix>` to `Results/SimulationResults/<DateSuffix>`.
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/PopulationParameters.xlsx
+++ b/tests/data/TestProject/Parameters/PopulationParameters.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/Services/Freigegebene Dokumente/_Project_template_V02.00/WP1_V00.01/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_3A82F05DCDDED6DECC8108D2AAE166FCA5131A3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D9440E7-2BDE-40B7-BCBC-A35A92C4F916}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B8C94-13CA-4464-A6AD-FE203ECC14C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9190" yWindow="430" windowWidth="28800" windowHeight="15290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="UserDefinedVariability" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -450,26 +450,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -533,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -565,16 +564,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDC7527-4ED0-4425-B4F9-CA5C81A120DE}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -866,6 +865,8 @@
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -879,5 +880,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B86647EE-866F-4D07-B65C-304BD8EB10F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B86647EE-866F-4D07-B65C-304BD8EB10F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>